<commit_message>
:pen: fix versions undefined and dates
</commit_message>
<xml_diff>
--- a/data/versiones.xlsx
+++ b/data/versiones.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caesar\Desktop\comentarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caesar\Desktop\comentarios\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4088762C-6C03-4636-8746-66BAD882B95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBAE29C-2870-417C-B831-F6BABE1DD15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="0" windowWidth="14430" windowHeight="15480" xr2:uid="{93E43FDB-A000-4BD5-BCD7-A99C2BF47BBF}"/>
+    <workbookView xWindow="14340" yWindow="0" windowWidth="14430" windowHeight="15480" xr2:uid="{93E43FDB-A000-4BD5-BCD7-A99C2BF47BBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="54">
   <si>
     <t>Cliente</t>
   </si>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t xml:space="preserve">220509 PLATAFORMADO PAX PUP 10 A35-ECOPAPAYNET </t>
-  </si>
-  <si>
-    <t>A920PRO</t>
   </si>
   <si>
     <t>220406 PLATAFORMADO PAX PUP 80 A920PRO - ECOPAYNET</t>
@@ -204,7 +201,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,6 +240,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -258,7 +263,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -327,12 +332,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -362,6 +382,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -679,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3B14F2-FDC4-4AC1-A44C-F888069A7F99}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,10 +963,10 @@
         <v>32</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -957,7 +983,7 @@
         <v>14</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -968,13 +994,13 @@
         <v>44678</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -985,13 +1011,13 @@
         <v>44669</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E18" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1005,7 +1031,7 @@
         <v>7009</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>12</v>
@@ -1019,10 +1045,10 @@
         <v>44669</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>12</v>
@@ -1039,7 +1065,7 @@
         <v>7009</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>12</v>
@@ -1047,7 +1073,7 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="4">
         <v>44804</v>
@@ -1057,7 +1083,7 @@
         <v>14</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1069,10 +1095,10 @@
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1082,13 +1108,13 @@
       <c r="B24" s="9"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E24" s="9"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="4">
         <v>44854</v>
@@ -1105,7 +1131,7 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B26" s="4">
         <v>44830</v>
@@ -1117,7 +1143,7 @@
         <v>23</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1131,15 +1157,15 @@
         <v>5</v>
       </c>
       <c r="D27" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="6" t="s">
+    </row>
+    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="B28" s="4">
         <v>44858</v>
@@ -1151,8 +1177,11 @@
         <v>14</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>53</v>
-      </c>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>